<commit_message>
(CENSORED data) **Need Guidance**  Added wy2016-17 Spillway pMeHg  folder; Updated pMeHg model results file for wy2016-17; Updated the Spillway Q and WQ worksheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_pMeHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_pMeHg Model Results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F6DFF3A-E6FE-4EC7-8D1E-441D50CEEF5E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BBDF99D9-2EE7-47DA-AD90-D49A84CF2066}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="pTHg wy2016-17 Model Results" sheetId="2" r:id="rId1"/>
+    <sheet name="pMeHg wy2016-17 Model Results" sheetId="2" r:id="rId1"/>
     <sheet name="Inlet" sheetId="3" r:id="rId2"/>
     <sheet name="Spillway" sheetId="4" r:id="rId3"/>
     <sheet name="Outlet" sheetId="5" r:id="rId4"/>
@@ -23,8 +23,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Rose, Shanna Lynn</author>
+  </authors>
+  <commentList>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{879746E8-978C-46FB-ABEF-1F9E00C10808}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rose, Shanna Lynn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There are 4 censored values for this parameter. Used one-half of the MDL (0.10 ng/L, so 0.05 ng/L for censored) in the data calculations for the constituent text file.
+-12/2/18</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="468">
   <si>
     <t>Model #</t>
   </si>
@@ -888,13 +923,553 @@
   </si>
   <si>
     <t>Number of Uncensored Observations: 32;  Period of record: 2016-01-07 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym1 &lt;- loadReg(pMeHg ~model(1), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 23</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 6.6765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Period of record: 2016-01-24 to 2017-04-04</t>
+  </si>
+  <si>
+    <t>(Intercept)   -7.738    0.18698  -41.39       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.312    0.08932   14.69       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5446</t>
+  </si>
+  <si>
+    <t>R-squared: 91.13 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 55.73 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.5124</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min 25% 50%  75%  90%  95%  Max</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.02 0.02 0.02 0.02</t>
+  </si>
+  <si>
+    <t>Obs   0   0   0 0.02 0.02 0.02 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -8.877 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7565</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym2 &lt;- loadReg(pMeHg ~model(2), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym2</t>
+  </si>
+  <si>
+    <t>(Intercept)  -8.4333    0.23733 -35.535   0e+00</t>
+  </si>
+  <si>
+    <t>lnQ           1.3123    0.07027  18.675   0e+00</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1586    0.04249   3.732   5e-04</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3371</t>
+  </si>
+  <si>
+    <t>R-squared: 94.77 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 67.88 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.5199</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2582</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.02 0.03 0.04 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 14.07 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.6558</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym3 &lt;- loadReg(pMeHg ~model(3), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym3</t>
+  </si>
+  <si>
+    <t>(Intercept)  -7.8018    0.16852 -46.296  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2408    0.08446  14.692  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME       0.8794    0.34664   2.537  0.0113</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.4326</t>
+  </si>
+  <si>
+    <t>R-squared: 93.29 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 62.15 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1062</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.1389</t>
+  </si>
+  <si>
+    <t>lnQ     1.126</t>
+  </si>
+  <si>
+    <t>DECTIME 1.126</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.02 0.02 0.02 0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -4.511 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7548</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym4 &lt;- loadReg(pMeHg ~model(4), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym4</t>
+  </si>
+  <si>
+    <t>(Intercept)   -2.550    1.68225  -1.516  0.1051</t>
+  </si>
+  <si>
+    <t>lnQ            1.404    0.08903  15.770  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   -4.472    1.35359  -3.304  0.0012</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   -4.012    1.42505  -2.815  0.0046</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.367</t>
+  </si>
+  <si>
+    <t>R-squared: 94.6 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 67.11 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.8443</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               VIF</t>
+  </si>
+  <si>
+    <t>lnQ          1.475</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 11.839</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.239</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.04 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -2.682 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7706</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym5 &lt;- loadReg(pMeHg ~model(5), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym5</t>
+  </si>
+  <si>
+    <t>(Intercept)  -8.3385    0.24623 -33.865  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.2775    0.07478  17.082  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1299    0.04785   2.715  0.0060</t>
+  </si>
+  <si>
+    <t>DECTIME       0.4286    0.34455   1.244  0.1796</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3281</t>
+  </si>
+  <si>
+    <t>R-squared: 95.17 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 69.68 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.8493</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3326</t>
+  </si>
+  <si>
+    <t>lnQ     1.163</t>
+  </si>
+  <si>
+    <t>lnQ2    1.303</t>
+  </si>
+  <si>
+    <t>DECTIME 1.466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.6814</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym6 &lt;- loadReg(pMeHg ~model(6), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym6</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.6488    1.25786  -2.901   3e-03</t>
+  </si>
+  <si>
+    <t>lnQ           1.4061    0.06511  21.595   0e+00</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1386    0.03311   4.187   1e-04</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -3.9651    0.99724  -3.976   1e-04</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -3.7213    1.04442  -3.563   5e-04</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1962</t>
+  </si>
+  <si>
+    <t>R-squared: 97.26 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.75 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7025</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.1892</t>
+  </si>
+  <si>
+    <t>lnQ2         1.043</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 12.016</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.297</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.06 0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 16.6 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.413</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym7 &lt;- loadReg(pMeHg ~model(7), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.2922    1.68324  -1.956  0.0353</t>
+  </si>
+  <si>
+    <t>lnQ           1.3596    0.09005  15.099  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME       0.5581    0.34981   1.595  0.0812</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -3.7634    1.37543  -2.736  0.0047</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -3.5801    1.39687  -2.563  0.0075</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3394</t>
+  </si>
+  <si>
+    <t>R-squared: 95.26 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 70.15 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2147</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.0423</t>
+  </si>
+  <si>
+    <t>lnQ          1.631</t>
+  </si>
+  <si>
+    <t>DECTIME      1.461</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 13.218</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -4.597 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8438</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym8 &lt;- loadReg(pMeHg ~model(8), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym8</t>
+  </si>
+  <si>
+    <t>(Intercept) -3.71454    1.32025 -2.8135  0.0030</t>
+  </si>
+  <si>
+    <t>lnQ          1.40012    0.07127 19.6461  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.13448    0.03804  3.5355  0.0004</t>
+  </si>
+  <si>
+    <t>DECTIME      0.07406    0.30562  0.2423  0.7782</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -3.88619    1.07496 -3.6152  0.0003</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -3.67266    1.09146 -3.3649  0.0006</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.2071</t>
+  </si>
+  <si>
+    <t>R-squared: 97.27 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.83 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6205</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.159</t>
+  </si>
+  <si>
+    <t>lnQ          1.674</t>
+  </si>
+  <si>
+    <t>lnQ2         1.305</t>
+  </si>
+  <si>
+    <t>DECTIME      1.828</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 13.232</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.763</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.05 0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 15.62 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.4682</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym9 &lt;- loadReg(pMeHg ~model(9), data = pMeHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Spillwaym9</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.9084    1.25919  -3.104  0.0010</t>
+  </si>
+  <si>
+    <t>lnQ           1.2854    0.09596  13.395  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1708    0.04204   4.062  0.0001</t>
+  </si>
+  <si>
+    <t>DECTIME       0.3386    0.32991   1.026  0.2260</t>
+  </si>
+  <si>
+    <t>DECTIME2     -5.1156    3.03251  -1.687  0.0523</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -2.6594    1.25349  -2.122  0.0169</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -2.9818    1.11461  -2.675  0.0035</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.1868</t>
+  </si>
+  <si>
+    <t>R-squared: 97.68 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 86.6 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1036</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.139</t>
+  </si>
+  <si>
+    <t>lnQ          3.365</t>
+  </si>
+  <si>
+    <t>lnQ2         1.767</t>
+  </si>
+  <si>
+    <t>DECTIME      2.361</t>
+  </si>
+  <si>
+    <t>DECTIME2     4.110</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 19.946</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 15.911</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.02 0.02 0.05 0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 15.54 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.493</t>
+  </si>
+  <si>
+    <t>&gt; View(pMeHg_Spillway)</t>
+  </si>
+  <si>
+    <t>x- cna selected</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 23; Period of record: 2016-01-24 to 2017-04-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,8 +1536,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1002,6 +1590,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1121,7 +1715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1207,6 +1801,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1214,6 +1811,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,80 +1834,20 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1763,7 +2309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1771,7 +2317,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1785,10 +2331,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>21</v>
@@ -1827,24 +2373,24 @@
       <c r="L2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="35"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
       <c r="Z4" s="18" t="s">
         <v>51</v>
       </c>
@@ -1859,21 +2405,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="32" t="s">
         <v>287</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="30" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="30"/>
+      <c r="L5" s="31"/>
       <c r="Z5" s="18" t="s">
         <v>52</v>
       </c>
@@ -1970,7 +2516,7 @@
         <v>0.54569999999999996</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>8</v>
+        <v>466</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -2031,43 +2577,43 @@
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="6">
         <v>0</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="28">
         <v>0.19120000000000001</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="6">
         <v>90.07</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="6">
         <v>0.13980000000000001</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="6">
         <v>2.2410000000000001</v>
       </c>
       <c r="L9" s="29">
         <v>0.59989999999999999</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N9" s="8" t="s">
@@ -2081,43 +2627,43 @@
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="A10" s="6">
         <v>4</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="6">
         <v>0</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="11">
         <v>0.1047</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="6">
         <v>9.7600000000000006E-2</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="6">
         <v>90.42</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="6">
         <v>0.25140000000000001</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="6">
         <v>5.52</v>
       </c>
       <c r="L10" s="29">
         <v>0.51060000000000005</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N10" s="8" t="s">
@@ -2371,34 +2917,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="30" t="s">
+      <c r="B18" s="42" t="s">
+        <v>467</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="30"/>
+      <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -2448,7 +2996,7 @@
       <c r="A20" s="29">
         <v>1</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="6">
         <v>0</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2466,13 +3014,21 @@
       <c r="G20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="I20" s="30">
+        <v>91.13</v>
+      </c>
+      <c r="J20" s="30">
+        <v>0.2036</v>
+      </c>
+      <c r="K20" s="30">
+        <v>-8.8770000000000007</v>
+      </c>
+      <c r="L20" s="30">
+        <v>0.75649999999999995</v>
+      </c>
       <c r="M20" s="29"/>
       <c r="N20" s="8" t="s">
         <v>17</v>
@@ -2488,10 +3044,12 @@
       <c r="A21" s="29">
         <v>2</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="6">
         <v>0</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="25">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="D21" s="10" t="s">
         <v>16</v>
       </c>
@@ -2504,13 +3062,21 @@
       <c r="G21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="I21" s="30">
+        <v>94.77</v>
+      </c>
+      <c r="J21" s="30">
+        <v>0.25819999999999999</v>
+      </c>
+      <c r="K21" s="30">
+        <v>14.07</v>
+      </c>
+      <c r="L21" s="30">
+        <v>0.65580000000000005</v>
+      </c>
       <c r="M21" s="29"/>
       <c r="N21" s="8" t="s">
         <v>17</v>
@@ -2526,13 +3092,15 @@
       <c r="A22" s="29">
         <v>3</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="6">
         <v>0</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="23"/>
+      <c r="D22" s="23">
+        <v>1.1299999999999999E-2</v>
+      </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
       </c>
@@ -2542,13 +3110,21 @@
       <c r="G22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="I22" s="30">
+        <v>93.29</v>
+      </c>
+      <c r="J22" s="30">
+        <v>0.1389</v>
+      </c>
+      <c r="K22" s="30">
+        <v>-4.5110000000000001</v>
+      </c>
+      <c r="L22" s="30">
+        <v>0.75480000000000003</v>
+      </c>
       <c r="M22" s="29"/>
       <c r="N22" s="8" t="s">
         <v>17</v>
@@ -2561,31 +3137,45 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23" s="29">
+      <c r="A23" s="11">
         <v>4</v>
       </c>
       <c r="B23" s="11">
         <v>0</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="29"/>
+      <c r="F23" s="11">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="G23" s="11">
+        <v>4.5999999999999999E-3</v>
+      </c>
       <c r="H23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
+      <c r="I23" s="11">
+        <v>94.6</v>
+      </c>
+      <c r="J23" s="11">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="K23" s="11">
+        <v>-2.6819999999999999</v>
+      </c>
+      <c r="L23" s="30">
+        <v>0.77059999999999995</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N23" s="8" t="s">
         <v>17</v>
       </c>
@@ -2600,11 +3190,15 @@
       <c r="A24" s="29">
         <v>5</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="6">
         <v>0</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="30">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D24" s="30">
+        <v>0.17960000000000001</v>
+      </c>
       <c r="E24" s="10" t="s">
         <v>16</v>
       </c>
@@ -2614,13 +3208,21 @@
       <c r="G24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="I24" s="30">
+        <v>95.17</v>
+      </c>
+      <c r="J24" s="30">
+        <v>0.33260000000000001</v>
+      </c>
+      <c r="K24" s="30">
+        <v>12</v>
+      </c>
+      <c r="L24" s="30">
+        <v>0.68140000000000001</v>
+      </c>
       <c r="M24" s="29"/>
       <c r="N24" s="8" t="s">
         <v>17</v>
@@ -2636,25 +3238,39 @@
       <c r="A25" s="29">
         <v>6</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="6">
         <v>0</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="25">
+        <v>1E-4</v>
+      </c>
       <c r="D25" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="11" t="s">
+      <c r="F25" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="G25" s="25">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="I25" s="30">
+        <v>97.26</v>
+      </c>
+      <c r="J25" s="30">
+        <v>-0.18920000000000001</v>
+      </c>
+      <c r="K25" s="30">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="L25" s="30">
+        <v>0.41299999999999998</v>
+      </c>
       <c r="M25" s="29"/>
       <c r="N25" s="8" t="s">
         <v>17</v>
@@ -2667,29 +3283,45 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="29">
+      <c r="A26" s="11">
         <v>7</v>
       </c>
       <c r="B26" s="11">
         <v>0</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="10" t="s">
+      <c r="D26" s="11">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="E26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="29"/>
+      <c r="F26" s="11">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="G26" s="11">
+        <v>7.4999999999999997E-3</v>
+      </c>
       <c r="H26" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
+      <c r="I26" s="11">
+        <v>95.26</v>
+      </c>
+      <c r="J26" s="11">
+        <v>-4.2299999999999997E-2</v>
+      </c>
+      <c r="K26" s="11">
+        <v>-4.5970000000000004</v>
+      </c>
+      <c r="L26" s="30">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N26" s="8" t="s">
         <v>17</v>
       </c>
@@ -2704,23 +3336,39 @@
       <c r="A27" s="29">
         <v>8</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="6">
         <v>0</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.7782</v>
+      </c>
       <c r="E27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="11" t="s">
+      <c r="F27" s="6">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G27" s="6">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
+      <c r="I27" s="30">
+        <v>97.27</v>
+      </c>
+      <c r="J27" s="30">
+        <v>-0.159</v>
+      </c>
+      <c r="K27" s="30">
+        <v>15.62</v>
+      </c>
+      <c r="L27" s="30">
+        <v>0.46820000000000001</v>
+      </c>
       <c r="M27" s="29"/>
       <c r="N27" s="8" t="s">
         <v>17</v>
@@ -2736,21 +3384,39 @@
       <c r="A28" s="29">
         <v>9</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="6">
         <v>0</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="11" t="s">
+      <c r="C28" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="E28" s="6">
+        <v>5.2299999999999999E-2</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
+      <c r="I28" s="30">
+        <v>97.68</v>
+      </c>
+      <c r="J28" s="30">
+        <v>-0.13900000000000001</v>
+      </c>
+      <c r="K28" s="30">
+        <v>15.54</v>
+      </c>
+      <c r="L28" s="30">
+        <v>0.49299999999999999</v>
+      </c>
       <c r="M28" s="29"/>
       <c r="N28" s="8" t="s">
         <v>17</v>
@@ -2763,34 +3429,34 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="40"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="30" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="30"/>
+      <c r="L31" s="31"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -3155,34 +3821,34 @@
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="37"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="30" t="s">
+      <c r="B44" s="32"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="30"/>
+      <c r="L44" s="31"/>
     </row>
     <row r="45" spans="1:27" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -3552,34 +4218,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="38" t="s">
+      <c r="B57" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="31"/>
+      <c r="L57" s="31"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="31"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="30" t="s">
+      <c r="B58" s="32"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="30"/>
+      <c r="L58" s="31"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -3839,27 +4505,27 @@
     <mergeCell ref="K44:L44"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
-    <cfRule type="cellIs" dxfId="17" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="36" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="37" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="38" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55 K60:K1048576 K57 K29">
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="22" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="23" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68">
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="19" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3890,6 +4556,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6365,118 +7032,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1DE6A6-09B0-4386-8D01-5CB04D0F065F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:A529"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29:H30"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -6485,1471 +7213,2285 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="13"/>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A526" s="15"/>
+      <c r="A526" s="15" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" s="16"/>

</xml_diff>

<commit_message>
(CENSORED data) Added wy2016-17 Combined Outflow pMeHg  folder;  Updated pMeHg model results file for wy2016-17;  Updated the Combined Outflow Q and WQ worksheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_pMeHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_pMeHg Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{095C065C-8676-4C64-844C-0FE8E94820C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{665015D7-415C-406C-87FD-E148676E921E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,12 +79,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{B6A99EBC-6F98-4B53-849D-C4B38DB5CCC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rose, Shanna Lynn:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+There are 5 censored values for this parameter. Used one-half of the MDL (0.10 ng/L, so 0.05 ng/L for censored) in the data calculations for the constituent text file.
+-12/3/18</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="819">
   <si>
     <t>Model #</t>
   </si>
@@ -2034,6 +2059,513 @@
   </si>
   <si>
     <t>Number of Uncensored Observations: 29; Period of record: 2016-01-20 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm1 &lt;- loadReg(pMeHg ~model(1), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 34</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0699</t>
+  </si>
+  <si>
+    <t>(Intercept)   -7.047    0.12634  -55.78       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.266    0.07596   16.66       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5316</t>
+  </si>
+  <si>
+    <t>R-squared: 89.66 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.16 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.4211</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3103</t>
+  </si>
+  <si>
+    <t>Est   0   0   0 0.01 0.02 0.02 0.02</t>
+  </si>
+  <si>
+    <t>Obs   0   0   0 0.01 0.02 0.02 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.6397 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8053</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm2 &lt;- loadReg(pMeHg ~model(2), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Estimate Std. Error   z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.0453442    0.20128 -35.00276   0.000</t>
+  </si>
+  <si>
+    <t>lnQ          1.2656286    0.07718  16.39863   0.000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.0006012    0.05605  -0.01073   0.991</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5487</t>
+  </si>
+  <si>
+    <t>G-squared: 77.16 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.4197</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.7838 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8047</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm3 &lt;- loadReg(pMeHg ~model(3), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)   -7.051    0.12717 -55.4470   0.000</t>
+  </si>
+  <si>
+    <t>lnQ            1.238    0.08409  14.7177   0.000</t>
+  </si>
+  <si>
+    <t>DECTIME        0.236    0.29537   0.7991   0.405</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5377</t>
+  </si>
+  <si>
+    <t>R-squared: 89.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.86 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6537</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.273</t>
+  </si>
+  <si>
+    <t>lnQ     1.211</t>
+  </si>
+  <si>
+    <t>DECTIME 1.211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 1.818 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.809</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm4 &lt;- loadReg(pMeHg ~model(4), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -5.8856    0.76926  -7.651  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.3176    0.08244  15.983  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.1471    0.66686  -1.720  0.0737</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.8267    0.65394  -1.264  0.1841</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5135</t>
+  </si>
+  <si>
+    <t>R-squared: 90.64 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 80.54 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6005</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2645</t>
+  </si>
+  <si>
+    <t>lnQ         1.219</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.817</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.874</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 3.892 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8821</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm5 &lt;- loadReg(pMeHg ~model(5), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept) -7.00293    0.20844 -33.5971  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.23377    0.08631  14.2942  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.01764    0.05985  -0.2948  0.7538</t>
+  </si>
+  <si>
+    <t>DECTIME      0.26786    0.31866   0.8406  0.3736</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.554</t>
+  </si>
+  <si>
+    <t>R-squared: 89.9 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.95 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6879</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2705</t>
+  </si>
+  <si>
+    <t>lnQ     1.239</t>
+  </si>
+  <si>
+    <t>lnQ2    1.130</t>
+  </si>
+  <si>
+    <t>DECTIME 1.368</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.4864 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8016</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm6 &lt;- loadReg(pMeHg ~model(6), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.69674    0.82317 -6.9205  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.32021    0.08326 15.8572  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.04307    0.06259 -0.6882  0.4580</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.27755    0.69896 -1.8278  0.0542</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.82439    0.65977 -1.2495  0.1818</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5227</t>
+  </si>
+  <si>
+    <t>G-squared: 81.09 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7195</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2455</t>
+  </si>
+  <si>
+    <t>lnQ         1.222</t>
+  </si>
+  <si>
+    <t>lnQ2        1.309</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.987 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8766</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm7 &lt;- loadReg(pMeHg ~model(7), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -5.5747     1.0082 -5.5295  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.3543     0.1125 12.0359  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.1917     0.3946 -0.4859  0.5996</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.4416     0.9075 -1.5885  0.0921</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -1.0532     0.8101 -1.3002  0.1652</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5269</t>
+  </si>
+  <si>
+    <t>R-squared: 90.72 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 80.81 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.3687</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.282</t>
+  </si>
+  <si>
+    <t>lnQ         2.213</t>
+  </si>
+  <si>
+    <t>DECTIME     2.206</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.888</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.793</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 3.705 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8873</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm8 &lt;- loadReg(pMeHg ~model(8), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.48828     1.0302 -5.3275  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.34693     0.1145 11.7659  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.03837     0.0650 -0.5902  0.5167</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.14132     0.4081 -0.3463  0.7031</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.48034     0.9202 -1.6087  0.0830</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.99163     0.8259 -1.2006  0.1914</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.539</t>
+  </si>
+  <si>
+    <t>R-squared: 90.83 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 81.23 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.4914</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2624</t>
+  </si>
+  <si>
+    <t>lnQ         2.240</t>
+  </si>
+  <si>
+    <t>lnQ2        1.369</t>
+  </si>
+  <si>
+    <t>DECTIME     2.307</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.924</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.887</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -0.5409 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8822</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm9 &lt;- loadReg(pMeHg ~model(9), data = pMeHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; pMeHg_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -5.45856    1.05024 -5.1975  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.37669    0.14448  9.5287  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.04356    0.06772 -0.6432  0.4721</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.22205    0.47544 -0.4671  0.6009</t>
+  </si>
+  <si>
+    <t>DECTIME2     0.76505    2.20355  0.3472  0.6972</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.69705    1.12423 -1.5095  0.0970</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -1.09689    0.89231 -1.2293  0.1736</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5565</t>
+  </si>
+  <si>
+    <t>R-squared: 90.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 81.38 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6616</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2646</t>
+  </si>
+  <si>
+    <t>lnQ          3.456</t>
+  </si>
+  <si>
+    <t>lnQ2         1.440</t>
+  </si>
+  <si>
+    <t>DECTIME      3.033</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.943</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 10.009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  6.656</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 0.5166 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8864</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34; Period of record: 2016-01-20 to 2017-04-26</t>
   </si>
 </sst>
 </file>
@@ -2293,7 +2825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2382,6 +2914,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2394,44 +2962,11 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2489,176 +3024,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3131,7 +3496,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3145,10 +3510,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>21</v>
@@ -3187,24 +3552,24 @@
       <c r="L2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="33"/>
+      <c r="O2" s="45"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
       <c r="Z4" s="18" t="s">
         <v>51</v>
       </c>
@@ -3219,21 +3584,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="42"/>
+      <c r="L5" s="34"/>
       <c r="Z5" s="18" t="s">
         <v>52</v>
       </c>
@@ -3731,36 +4096,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="38"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>458</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="42" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="42"/>
+      <c r="L18" s="34"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -4243,36 +4608,36 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="43"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="38" t="s">
         <v>649</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="42" t="s">
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="42"/>
+      <c r="L31" s="34"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -4720,7 +5085,7 @@
       <c r="E41" s="6">
         <v>0.82969999999999999</v>
       </c>
-      <c r="F41" s="46">
+      <c r="F41" s="33">
         <v>0.2898</v>
       </c>
       <c r="G41" s="6">
@@ -4753,34 +5118,36 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="38"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="43"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B44" s="39"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="42" t="s">
+      <c r="B44" s="38" t="s">
+        <v>818</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="42"/>
+      <c r="L44" s="34"/>
     </row>
     <row r="45" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -4827,35 +5194,45 @@
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A46" s="29">
+      <c r="A46" s="11">
         <v>1</v>
       </c>
       <c r="B46" s="11">
         <v>0</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
+      <c r="I46" s="11">
+        <v>89.66</v>
+      </c>
+      <c r="J46" s="11">
+        <v>0.31030000000000002</v>
+      </c>
+      <c r="K46" s="11">
+        <v>-0.63970000000000005</v>
+      </c>
+      <c r="L46" s="32">
+        <v>0.80530000000000002</v>
+      </c>
+      <c r="M46" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N46" s="8" t="s">
         <v>17</v>
       </c>
@@ -4870,10 +5247,12 @@
       <c r="A47" s="29">
         <v>2</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="6">
         <v>0</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="25">
+        <v>0.99099999999999999</v>
+      </c>
       <c r="D47" s="10" t="s">
         <v>16</v>
       </c>
@@ -4886,13 +5265,21 @@
       <c r="G47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
+      <c r="I47" s="32">
+        <v>89.66</v>
+      </c>
+      <c r="J47" s="32">
+        <v>0.3105</v>
+      </c>
+      <c r="K47" s="32">
+        <v>-0.78380000000000005</v>
+      </c>
+      <c r="L47" s="32">
+        <v>0.80469999999999997</v>
+      </c>
       <c r="M47" s="29"/>
       <c r="N47" s="8" t="s">
         <v>17</v>
@@ -4908,13 +5295,15 @@
       <c r="A48" s="29">
         <v>3</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="6">
         <v>0</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="23"/>
+      <c r="D48" s="23">
+        <v>0.40500000000000003</v>
+      </c>
       <c r="E48" s="10" t="s">
         <v>16</v>
       </c>
@@ -4924,13 +5313,21 @@
       <c r="G48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
+      <c r="I48" s="32">
+        <v>89.87</v>
+      </c>
+      <c r="J48" s="32">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="K48" s="32">
+        <v>1.8180000000000001</v>
+      </c>
+      <c r="L48" s="32">
+        <v>0.80900000000000005</v>
+      </c>
       <c r="M48" s="29"/>
       <c r="N48" s="8" t="s">
         <v>17</v>
@@ -4946,7 +5343,7 @@
       <c r="A49" s="29">
         <v>4</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -4958,15 +5355,27 @@
       <c r="E49" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="11" t="s">
+      <c r="F49" s="6">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="G49" s="32">
+        <v>0.18410000000000001</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
+      <c r="I49" s="33">
+        <v>90.64</v>
+      </c>
+      <c r="J49" s="32">
+        <v>0.26450000000000001</v>
+      </c>
+      <c r="K49" s="32">
+        <v>3.8919999999999999</v>
+      </c>
+      <c r="L49" s="32">
+        <v>0.8821</v>
+      </c>
       <c r="M49" s="29"/>
       <c r="N49" s="8" t="s">
         <v>17</v>
@@ -4982,11 +5391,15 @@
       <c r="A50" s="29">
         <v>5</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="6">
         <v>0</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
+      <c r="C50" s="32">
+        <v>0.75380000000000003</v>
+      </c>
+      <c r="D50" s="32">
+        <v>0.37359999999999999</v>
+      </c>
       <c r="E50" s="10" t="s">
         <v>16</v>
       </c>
@@ -4996,13 +5409,21 @@
       <c r="G50" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H50" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
+      <c r="I50" s="32">
+        <v>89.9</v>
+      </c>
+      <c r="J50" s="32">
+        <v>0.27050000000000002</v>
+      </c>
+      <c r="K50" s="32">
+        <v>-0.4864</v>
+      </c>
+      <c r="L50" s="32">
+        <v>0.80159999999999998</v>
+      </c>
       <c r="M50" s="29"/>
       <c r="N50" s="8" t="s">
         <v>17</v>
@@ -5018,25 +5439,39 @@
       <c r="A51" s="29">
         <v>6</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="6">
         <v>0</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="32">
+        <v>0.45800000000000002</v>
+      </c>
       <c r="D51" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="11" t="s">
+      <c r="F51" s="6">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="G51" s="32">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
+      <c r="I51" s="32">
+        <v>90.79</v>
+      </c>
+      <c r="J51" s="32">
+        <v>0.2455</v>
+      </c>
+      <c r="K51" s="32">
+        <v>-0.98699999999999999</v>
+      </c>
+      <c r="L51" s="32">
+        <v>0.87660000000000005</v>
+      </c>
       <c r="M51" s="29"/>
       <c r="N51" s="8" t="s">
         <v>17</v>
@@ -5052,25 +5487,39 @@
       <c r="A52" s="29">
         <v>7</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="6">
         <v>0</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6">
+        <v>0.59960000000000002</v>
+      </c>
       <c r="E52" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="11" t="s">
+      <c r="F52" s="6">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="G52" s="32">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
+      <c r="I52" s="32">
+        <v>90.72</v>
+      </c>
+      <c r="J52" s="32">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="K52" s="32">
+        <v>3.7050000000000001</v>
+      </c>
+      <c r="L52" s="32">
+        <v>0.88729999999999998</v>
+      </c>
       <c r="M52" s="29"/>
       <c r="N52" s="8" t="s">
         <v>17</v>
@@ -5086,23 +5535,39 @@
       <c r="A53" s="29">
         <v>8</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="6">
         <v>0</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="32">
+        <v>0.51670000000000005</v>
+      </c>
+      <c r="D53" s="32">
+        <v>0.70309999999999995</v>
+      </c>
       <c r="E53" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="11" t="s">
+      <c r="F53" s="6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.19139999999999999</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
+      <c r="I53" s="32">
+        <v>90.83</v>
+      </c>
+      <c r="J53" s="32">
+        <v>0.26240000000000002</v>
+      </c>
+      <c r="K53" s="32">
+        <v>-0.54090000000000005</v>
+      </c>
+      <c r="L53" s="32">
+        <v>0.88219999999999998</v>
+      </c>
       <c r="M53" s="29"/>
       <c r="N53" s="8" t="s">
         <v>17</v>
@@ -5118,21 +5583,39 @@
       <c r="A54" s="29">
         <v>9</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="6">
         <v>0</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="11" t="s">
+      <c r="C54" s="32">
+        <v>0.47210000000000002</v>
+      </c>
+      <c r="D54" s="6">
+        <v>0.60089999999999999</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="F54" s="6">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.1736</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
+      <c r="I54" s="32">
+        <v>90.87</v>
+      </c>
+      <c r="J54" s="32">
+        <v>0.2646</v>
+      </c>
+      <c r="K54" s="32">
+        <v>0.51659999999999995</v>
+      </c>
+      <c r="L54" s="32">
+        <v>0.88639999999999997</v>
+      </c>
       <c r="M54" s="29"/>
       <c r="N54" s="8" t="s">
         <v>17</v>
@@ -5150,34 +5633,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="42"/>
-      <c r="L57" s="42"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="39"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="42" t="s">
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="36"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="42"/>
+      <c r="L58" s="34"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -5417,6 +5900,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K58:L58"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B18:J18"/>
@@ -5429,74 +5918,73 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="K44:L44"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="40" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="41" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="42" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55 K60:K1048576 K57 K29">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="26" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="27" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46:L54 L33:L41 L20:L28 L7:L15">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:K54 K33:K35 K20:K28 K7:K15 K37:K41">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="K46:K52 K33:K35 K20:K28 K7:K15 K37:K41 K54">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54 C34 D35 C37:C38 D37 C40:C41 D39:D41 E41 F36:G36 F38:G40 C21 D22 C24:C25 D24 C27:C28 D26:D28 E28 F23:G23 F25:G28 C8 D9 C11:C12 D11 C14:C15 D13:D15 E15 F10:G10 F12:G15 G41">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52 F49:G49 F51:G54 C34 D35 C37:C38 D37 C40:C41 D39:D41 E41 F36:G36 F38:G40 C21 D22 C24:C25 D24 C27:C28 D26:D28 E28 F23:G23 F25:G28 C8 D9 C11:C12 D11 C14:C15 D13:D15 E15 F10:G10 F12:G15 G41 D54:E54">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12933,118 +13421,179 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FBE2AD-EC1E-4563-8289-C8C08DD23DD5}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:A528"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -13053,1465 +13602,2277 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="16"/>

</xml_diff>